<commit_message>
updating words which dont display properly
</commit_message>
<xml_diff>
--- a/Assignment3/dataset/hi_conditions.xlsx
+++ b/Assignment3/dataset/hi_conditions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="185">
   <si>
     <t xml:space="preserve">hword1</t>
   </si>
@@ -43,10 +43,10 @@
     <t xml:space="preserve">right</t>
   </si>
   <si>
-    <t xml:space="preserve">मगरमच्छ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crocodile</t>
+    <t xml:space="preserve">शेर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lion</t>
   </si>
   <si>
     <t xml:space="preserve">गाड़ी</t>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">auto</t>
   </si>
   <si>
-    <t xml:space="preserve">बच्चा</t>
+    <t xml:space="preserve">लड़की</t>
   </si>
   <si>
     <t xml:space="preserve">baby</t>
@@ -73,13 +73,13 @@
     <t xml:space="preserve">beast</t>
   </si>
   <si>
-    <t xml:space="preserve">विज्ञान</t>
+    <t xml:space="preserve">गणित</t>
   </si>
   <si>
     <t xml:space="preserve">biology</t>
   </si>
   <si>
-    <t xml:space="preserve">विस्फोट</t>
+    <t xml:space="preserve">आतंकवादी</t>
   </si>
   <si>
     <t xml:space="preserve">bomb</t>
@@ -97,9 +97,6 @@
     <t xml:space="preserve">boxer</t>
   </si>
   <si>
-    <t xml:space="preserve">लड़की</t>
-  </si>
-  <si>
     <t xml:space="preserve">boy</t>
   </si>
   <si>
@@ -115,7 +112,7 @@
     <t xml:space="preserve">cash</t>
   </si>
   <si>
-    <t xml:space="preserve">महंगी</t>
+    <t xml:space="preserve">महंगा</t>
   </si>
   <si>
     <t xml:space="preserve">cheap</t>
@@ -127,10 +124,10 @@
     <t xml:space="preserve">china</t>
   </si>
   <si>
-    <t xml:space="preserve">मंदिर</t>
-  </si>
-  <si>
-    <t xml:space="preserve">church</t>
+    <t xml:space="preserve">भगवान</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temple</t>
   </si>
   <si>
     <t xml:space="preserve">पागल</t>
@@ -163,7 +160,7 @@
     <t xml:space="preserve">diamond</t>
   </si>
   <si>
-    <t xml:space="preserve">कृषि</t>
+    <t xml:space="preserve">खेती</t>
   </si>
   <si>
     <t xml:space="preserve">dollars</t>
@@ -184,7 +181,7 @@
     <t xml:space="preserve">employer</t>
   </si>
   <si>
-    <t xml:space="preserve">तथ्य</t>
+    <t xml:space="preserve">सच</t>
   </si>
   <si>
     <t xml:space="preserve">copy</t>
@@ -196,13 +193,13 @@
     <t xml:space="preserve">blush</t>
   </si>
   <si>
-    <t xml:space="preserve">योद्धा</t>
+    <t xml:space="preserve">सिपाही</t>
   </si>
   <si>
     <t xml:space="preserve">empty</t>
   </si>
   <si>
-    <t xml:space="preserve">चलचित्र</t>
+    <t xml:space="preserve">घर</t>
   </si>
   <si>
     <t xml:space="preserve">blow</t>
@@ -232,19 +229,19 @@
     <t xml:space="preserve">area</t>
   </si>
   <si>
-    <t xml:space="preserve">जंगल</t>
+    <t xml:space="preserve">वन</t>
   </si>
   <si>
     <t xml:space="preserve">chaos</t>
   </si>
   <si>
-    <t xml:space="preserve">नाजुक</t>
+    <t xml:space="preserve">कोमल</t>
   </si>
   <si>
     <t xml:space="preserve">cure</t>
   </si>
   <si>
-    <t xml:space="preserve">राक्षस</t>
+    <t xml:space="preserve">अभिनय</t>
   </si>
   <si>
     <t xml:space="preserve">calm</t>
@@ -274,7 +271,7 @@
     <t xml:space="preserve">deaf</t>
   </si>
   <si>
-    <t xml:space="preserve">कार्य</t>
+    <t xml:space="preserve">काम</t>
   </si>
   <si>
     <t xml:space="preserve">imhge</t>
@@ -283,9 +280,6 @@
     <t xml:space="preserve">left</t>
   </si>
   <si>
-    <t xml:space="preserve">अभिनेत्री</t>
-  </si>
-  <si>
     <t xml:space="preserve">disbhvmeve</t>
   </si>
   <si>
@@ -295,13 +289,13 @@
     <t xml:space="preserve">mabapine</t>
   </si>
   <si>
-    <t xml:space="preserve">समझौता</t>
+    <t xml:space="preserve">बातचीत</t>
   </si>
   <si>
     <t xml:space="preserve">busg</t>
   </si>
   <si>
-    <t xml:space="preserve">चेतावनी</t>
+    <t xml:space="preserve">सावधान</t>
   </si>
   <si>
     <t xml:space="preserve">caklqblower</t>
@@ -313,13 +307,13 @@
     <t xml:space="preserve">sastir</t>
   </si>
   <si>
-    <t xml:space="preserve">चींटी</t>
+    <t xml:space="preserve">खटमल</t>
   </si>
   <si>
     <t xml:space="preserve">rntractr</t>
   </si>
   <si>
-    <t xml:space="preserve">डिब्बा</t>
+    <t xml:space="preserve">पेटी</t>
   </si>
   <si>
     <t xml:space="preserve">tomer</t>
@@ -349,13 +343,13 @@
     <t xml:space="preserve">poldcemps</t>
   </si>
   <si>
-    <t xml:space="preserve">बाल्टी</t>
+    <t xml:space="preserve">नल</t>
   </si>
   <si>
     <t xml:space="preserve">ltbster</t>
   </si>
   <si>
-    <t xml:space="preserve">भेंस</t>
+    <t xml:space="preserve">गाय</t>
   </si>
   <si>
     <t xml:space="preserve">valuabzr</t>
@@ -365,9 +359,6 @@
   </si>
   <si>
     <t xml:space="preserve">dasewn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">सतर्क</t>
   </si>
   <si>
     <t xml:space="preserve">capmpiwity</t>
@@ -598,6 +589,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -618,11 +610,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Lohit Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -667,7 +661,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -677,6 +671,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -699,8 +697,8 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -864,10 +862,10 @@
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>6</v>
@@ -878,10 +876,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>
@@ -892,10 +890,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -906,10 +904,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
@@ -920,10 +918,10 @@
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
@@ -934,10 +932,10 @@
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
@@ -948,10 +946,10 @@
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>6</v>
@@ -962,10 +960,10 @@
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>6</v>
@@ -976,10 +974,10 @@
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
@@ -990,10 +988,10 @@
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -1004,10 +1002,10 @@
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
@@ -1018,10 +1016,10 @@
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
@@ -1032,10 +1030,10 @@
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
@@ -1046,10 +1044,10 @@
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
@@ -1060,10 +1058,10 @@
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
@@ -1074,10 +1072,10 @@
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -1088,10 +1086,10 @@
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>6</v>
@@ -1102,10 +1100,10 @@
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
@@ -1116,10 +1114,10 @@
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -1130,10 +1128,10 @@
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -1144,10 +1142,10 @@
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
@@ -1158,10 +1156,10 @@
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
@@ -1172,10 +1170,10 @@
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>6</v>
@@ -1186,10 +1184,10 @@
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>6</v>
@@ -1200,10 +1198,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>6</v>
@@ -1214,10 +1212,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>6</v>
@@ -1228,10 +1226,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>6</v>
@@ -1242,10 +1240,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>6</v>
@@ -1256,10 +1254,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>6</v>
@@ -1270,10 +1268,10 @@
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>6</v>
@@ -1282,15 +1280,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="C42" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>10</v>
@@ -1298,13 +1296,13 @@
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D43" s="1" t="n">
         <v>10</v>
@@ -1312,13 +1310,13 @@
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D44" s="1" t="n">
         <v>10</v>
@@ -1326,13 +1324,13 @@
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45" s="1" t="n">
         <v>10</v>
@@ -1340,13 +1338,13 @@
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D46" s="1" t="n">
         <v>10</v>
@@ -1354,13 +1352,13 @@
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D47" s="1" t="n">
         <v>10</v>
@@ -1368,13 +1366,13 @@
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D48" s="1" t="n">
         <v>10</v>
@@ -1382,13 +1380,13 @@
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>10</v>
@@ -1396,13 +1394,13 @@
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D50" s="1" t="n">
         <v>10</v>
@@ -1410,13 +1408,13 @@
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D51" s="1" t="n">
         <v>10</v>
@@ -1424,13 +1422,13 @@
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D52" s="1" t="n">
         <v>10</v>
@@ -1438,13 +1436,13 @@
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D53" s="1" t="n">
         <v>10</v>
@@ -1452,13 +1450,13 @@
     </row>
     <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D54" s="1" t="n">
         <v>10</v>
@@ -1466,13 +1464,13 @@
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D55" s="1" t="n">
         <v>10</v>
@@ -1480,13 +1478,13 @@
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D56" s="1" t="n">
         <v>10</v>
@@ -1494,13 +1492,13 @@
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>10</v>
@@ -1508,13 +1506,13 @@
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D58" s="1" t="n">
         <v>10</v>
@@ -1522,13 +1520,13 @@
     </row>
     <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>10</v>
@@ -1536,13 +1534,13 @@
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D60" s="1" t="n">
         <v>10</v>
@@ -1550,13 +1548,13 @@
     </row>
     <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>10</v>
@@ -1564,13 +1562,13 @@
     </row>
     <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>8</v>
@@ -1578,13 +1576,13 @@
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>8</v>
@@ -1592,13 +1590,13 @@
     </row>
     <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D64" s="1" t="n">
         <v>8</v>
@@ -1606,13 +1604,13 @@
     </row>
     <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D65" s="1" t="n">
         <v>8</v>
@@ -1620,13 +1618,13 @@
     </row>
     <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>8</v>
@@ -1634,13 +1632,13 @@
     </row>
     <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>8</v>
@@ -1648,13 +1646,13 @@
     </row>
     <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D68" s="1" t="n">
         <v>8</v>
@@ -1662,13 +1660,13 @@
     </row>
     <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D69" s="1" t="n">
         <v>8</v>
@@ -1676,13 +1674,13 @@
     </row>
     <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>8</v>
@@ -1690,13 +1688,13 @@
     </row>
     <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>8</v>
@@ -1704,13 +1702,13 @@
     </row>
     <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D72" s="1" t="n">
         <v>8</v>
@@ -1718,13 +1716,13 @@
     </row>
     <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D73" s="1" t="n">
         <v>8</v>
@@ -1732,13 +1730,13 @@
     </row>
     <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D74" s="1" t="n">
         <v>8</v>
@@ -1746,13 +1744,13 @@
     </row>
     <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D75" s="1" t="n">
         <v>8</v>
@@ -1760,13 +1758,13 @@
     </row>
     <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D76" s="1" t="n">
         <v>8</v>
@@ -1774,13 +1772,13 @@
     </row>
     <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D77" s="1" t="n">
         <v>8</v>
@@ -1788,13 +1786,13 @@
     </row>
     <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>8</v>
@@ -1802,13 +1800,13 @@
     </row>
     <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D79" s="1" t="n">
         <v>8</v>
@@ -1816,13 +1814,13 @@
     </row>
     <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D80" s="1" t="n">
         <v>8</v>
@@ -1830,13 +1828,13 @@
     </row>
     <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D81" s="1" t="n">
         <v>8</v>
@@ -1844,13 +1842,13 @@
     </row>
     <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D82" s="1" t="n">
         <v>9</v>
@@ -1858,13 +1856,13 @@
     </row>
     <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D83" s="1" t="n">
         <v>9</v>
@@ -1872,13 +1870,13 @@
     </row>
     <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D84" s="1" t="n">
         <v>9</v>
@@ -1886,13 +1884,13 @@
     </row>
     <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D85" s="1" t="n">
         <v>9</v>
@@ -1900,13 +1898,13 @@
     </row>
     <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D86" s="1" t="n">
         <v>9</v>
@@ -1914,13 +1912,13 @@
     </row>
     <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D87" s="1" t="n">
         <v>9</v>
@@ -1928,13 +1926,13 @@
     </row>
     <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D88" s="1" t="n">
         <v>9</v>
@@ -1942,13 +1940,13 @@
     </row>
     <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D89" s="1" t="n">
         <v>9</v>
@@ -1956,13 +1954,13 @@
     </row>
     <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D90" s="1" t="n">
         <v>9</v>
@@ -1970,13 +1968,13 @@
     </row>
     <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D91" s="1" t="n">
         <v>9</v>
@@ -1984,13 +1982,13 @@
     </row>
     <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D92" s="1" t="n">
         <v>9</v>
@@ -1998,13 +1996,13 @@
     </row>
     <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D93" s="1" t="n">
         <v>9</v>
@@ -2012,13 +2010,13 @@
     </row>
     <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D94" s="1" t="n">
         <v>9</v>
@@ -2026,13 +2024,13 @@
     </row>
     <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D95" s="1" t="n">
         <v>9</v>
@@ -2040,13 +2038,13 @@
     </row>
     <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D96" s="1" t="n">
         <v>9</v>
@@ -2054,13 +2052,13 @@
     </row>
     <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D97" s="1" t="n">
         <v>9</v>
@@ -2068,13 +2066,13 @@
     </row>
     <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D98" s="1" t="n">
         <v>9</v>
@@ -2082,13 +2080,13 @@
     </row>
     <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D99" s="1" t="n">
         <v>9</v>
@@ -2096,13 +2094,13 @@
     </row>
     <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D100" s="1" t="n">
         <v>9</v>
@@ -2110,13 +2108,13 @@
     </row>
     <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D101" s="1" t="n">
         <v>9</v>

</xml_diff>